<commit_message>
Lab2: passed all traces of essential commands
</commit_message>
<xml_diff>
--- a/lab2-single-cycle-cpu/数据通路表、控制信号取值表.xlsx
+++ b/lab2-single-cycle-cpu/数据通路表、控制信号取值表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25200" windowHeight="11990"/>
+    <workbookView windowWidth="25200" windowHeight="12030" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="数据通路表(含控制信号)" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="135">
   <si>
     <t>所属单元</t>
   </si>
@@ -212,7 +212,7 @@
     <t>beq</t>
   </si>
   <si>
-    <t>ALU.eq</t>
+    <t>ALU.comp</t>
   </si>
   <si>
     <t>IROM.inst[31 | 7 | 30:25 | 11:8]</t>
@@ -221,21 +221,12 @@
     <t>bne</t>
   </si>
   <si>
-    <t>ALU.ne</t>
-  </si>
-  <si>
     <t>blt</t>
   </si>
   <si>
-    <t>ALU.lt</t>
-  </si>
-  <si>
     <t>bge</t>
   </si>
   <si>
-    <t>ALU.ge</t>
-  </si>
-  <si>
     <t>U-类型</t>
   </si>
   <si>
@@ -255,12 +246,6 @@
   </si>
   <si>
     <t>完整</t>
-  </si>
-  <si>
-    <t>ALU.eq
-ALU.ne
-ALU.lt
-ALU.ge</t>
   </si>
   <si>
     <t>ALU.c
@@ -297,9 +282,6 @@
     <t>多路选择信号</t>
   </si>
   <si>
-    <t>npc_brsel</t>
-  </si>
-  <si>
     <t>rf_wsel</t>
   </si>
   <si>
@@ -321,9 +303,6 @@
     <t>控制信号</t>
   </si>
   <si>
-    <t>npc_br_sel</t>
-  </si>
-  <si>
     <t>0110011</t>
   </si>
   <si>
@@ -417,28 +396,16 @@
     <t>NPC_BRA</t>
   </si>
   <si>
-    <t>NPC_BR_EQ</t>
-  </si>
-  <si>
     <t>EXT_B</t>
   </si>
   <si>
     <t>ALU_EQ</t>
   </si>
   <si>
-    <t>NPC_BR_NE</t>
-  </si>
-  <si>
     <t>ALU_NE</t>
   </si>
   <si>
-    <t>NPC_BR_LT</t>
-  </si>
-  <si>
     <t>ALU_LT</t>
-  </si>
-  <si>
-    <t>NPC_BR_GE</t>
   </si>
   <si>
     <t>ALU_GE</t>
@@ -465,9 +432,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -492,6 +459,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -499,9 +474,70 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -515,16 +551,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -539,58 +567,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
@@ -607,7 +583,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -615,22 +598,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -651,7 +618,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -663,31 +630,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -699,7 +648,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -717,7 +672,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,19 +726,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -753,7 +768,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -765,73 +798,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -933,21 +900,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1001,6 +953,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1025,148 +992,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1567,28 +1534,28 @@
   <sheetPr/>
   <dimension ref="B2:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0714285714286" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="11.0692307692308" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.46428571428571" customWidth="1"/>
-    <col min="2" max="2" width="9.78571428571429" customWidth="1"/>
-    <col min="3" max="3" width="7.71428571428571" customWidth="1"/>
-    <col min="4" max="4" width="5.64285714285714" customWidth="1"/>
-    <col min="5" max="5" width="7.92857142857143" customWidth="1"/>
-    <col min="6" max="6" width="8.64285714285714" customWidth="1"/>
-    <col min="7" max="7" width="5.57142857142857" customWidth="1"/>
-    <col min="8" max="8" width="5.64285714285714" customWidth="1"/>
-    <col min="9" max="10" width="14.6428571428571" customWidth="1"/>
-    <col min="11" max="11" width="13.5" customWidth="1"/>
-    <col min="12" max="12" width="8.85714285714286" customWidth="1"/>
-    <col min="13" max="13" width="28.5714285714286" customWidth="1"/>
-    <col min="14" max="14" width="6.5" customWidth="1"/>
-    <col min="15" max="15" width="7.92857142857143" customWidth="1"/>
-    <col min="16" max="16" width="5.57142857142857" customWidth="1"/>
-    <col min="17" max="17" width="6.5" customWidth="1"/>
+    <col min="1" max="1" width="3.46153846153846" customWidth="1"/>
+    <col min="2" max="2" width="10.6153846153846" customWidth="1"/>
+    <col min="3" max="3" width="8.23076923076923" customWidth="1"/>
+    <col min="4" max="4" width="5.92307692307692" customWidth="1"/>
+    <col min="5" max="5" width="8.07692307692308" customWidth="1"/>
+    <col min="6" max="6" width="9.61538461538461" customWidth="1"/>
+    <col min="7" max="7" width="5.92307692307692" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
+    <col min="9" max="10" width="15.0769230769231" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="9.76923076923077" customWidth="1"/>
+    <col min="13" max="13" width="29.3846153846154" customWidth="1"/>
+    <col min="14" max="14" width="6.69230769230769" customWidth="1"/>
+    <col min="15" max="15" width="8.07692307692308" customWidth="1"/>
+    <col min="16" max="16" width="5.92307692307692" customWidth="1"/>
+    <col min="17" max="17" width="6.69230769230769" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17">
@@ -2797,7 +2764,7 @@
         <v>48</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>31</v>
@@ -2835,7 +2802,7 @@
     </row>
     <row r="30" spans="2:17">
       <c r="B30" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>29</v>
@@ -2847,7 +2814,7 @@
         <v>48</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>31</v>
@@ -2885,7 +2852,7 @@
     </row>
     <row r="31" spans="2:17">
       <c r="B31" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>29</v>
@@ -2897,7 +2864,7 @@
         <v>48</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>31</v>
@@ -2935,7 +2902,7 @@
     </row>
     <row r="32" spans="2:17">
       <c r="B32" s="13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -2955,7 +2922,7 @@
     </row>
     <row r="33" spans="2:17">
       <c r="B33" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>29</v>
@@ -2988,7 +2955,7 @@
         <v>48</v>
       </c>
       <c r="M33" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="N33" s="8" t="s">
         <v>31</v>
@@ -3005,7 +2972,7 @@
     </row>
     <row r="34" spans="2:17">
       <c r="B34" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
@@ -3025,7 +2992,7 @@
     </row>
     <row r="35" spans="2:17">
       <c r="B35" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>29</v>
@@ -3058,7 +3025,7 @@
         <v>58</v>
       </c>
       <c r="M35" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N35" s="8" t="s">
         <v>31</v>
@@ -3073,9 +3040,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" ht="66" spans="2:17">
+    <row r="36" ht="80" spans="2:17">
       <c r="B36" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>29</v>
@@ -3087,7 +3054,7 @@
         <v>48</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>35</v>
@@ -3105,16 +3072,16 @@
         <v>34</v>
       </c>
       <c r="L36" s="14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M36" s="14" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N36" s="8" t="s">
         <v>36</v>
       </c>
       <c r="O36" s="14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="P36" s="8" t="s">
         <v>35</v>
@@ -3125,13 +3092,13 @@
     </row>
     <row r="37" spans="2:17">
       <c r="B37" s="15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>31</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
@@ -3146,24 +3113,24 @@
         <v>31</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="L37" s="19"/>
       <c r="M37" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="N37" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="O37" s="19"/>
       <c r="P37" s="12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="Q37" s="19"/>
     </row>
     <row r="38" spans="2:17">
       <c r="B38" s="15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>31</v>
@@ -3174,8 +3141,8 @@
       <c r="E38" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="8" t="s">
-        <v>91</v>
+      <c r="F38" s="23" t="s">
+        <v>31</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>31</v>
@@ -3193,7 +3160,7 @@
         <v>31</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="M38" s="8" t="s">
         <v>31</v>
@@ -3202,7 +3169,7 @@
         <v>31</v>
       </c>
       <c r="O38" s="8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="P38" s="8" t="s">
         <v>31</v>
@@ -3240,44 +3207,43 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:M33"/>
+  <dimension ref="B2:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0714285714286" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="11.0692307692308" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.69285714285714" customWidth="1"/>
-    <col min="2" max="2" width="5.35714285714286" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.35714285714286" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.21428571428571" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.35714285714286" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.21428571428571" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.35714285714286" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28571428571429" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.21428571428571" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28571428571429" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.1428571428571" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.14285714285714" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.69230769230769" customWidth="1"/>
+    <col min="2" max="2" width="5.35384615384615" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.35384615384615" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.21538461538462" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.35384615384615" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21538461538461" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.35384615384615" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28461538461539" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.21538461538462" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28461538461539" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1461538461538" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.14615384615385" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13">
+    <row r="2" spans="2:12">
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -3285,39 +3251,35 @@
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-    </row>
-    <row r="3" spans="2:13">
+    </row>
+    <row r="3" spans="2:12">
       <c r="B3" s="2"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J3" s="10" t="s">
         <v>87</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>88</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
       <c r="B4" s="5" t="s">
         <v>27</v>
       </c>
@@ -3331,313 +3293,288 @@
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-    </row>
-    <row r="5" spans="2:13">
+    </row>
+    <row r="5" spans="2:12">
       <c r="B5" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K5" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="9">
-        <v>1</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="M5" s="9">
+      <c r="L5" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="2:12">
       <c r="B6" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="K6" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="9">
-        <v>1</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="M6" s="9">
+      <c r="L6" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:13">
+    <row r="7" spans="2:12">
       <c r="B7" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="9">
+        <v>1</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="9">
-        <v>1</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="M7" s="9">
+      <c r="L7" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:13">
+    <row r="8" spans="2:12">
       <c r="B8" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G8" s="9">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="K8" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="9">
-        <v>1</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="M8" s="9">
+      <c r="L8" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:13">
+    <row r="9" spans="2:12">
       <c r="B9" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="K9" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="9">
-        <v>1</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="M9" s="9">
+      <c r="L9" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:13">
+    <row r="10" spans="2:12">
       <c r="B10" s="7" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" s="9">
+        <v>1</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="K10" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="9">
-        <v>1</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="M10" s="9">
+      <c r="L10" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:13">
+    <row r="11" spans="2:12">
       <c r="B11" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G11" s="9">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="K11" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="9">
-        <v>1</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="M11" s="9">
+      <c r="L11" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:13">
+    <row r="12" spans="2:12">
       <c r="B12" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D12" s="8">
         <v>101</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="9">
+        <v>97</v>
+      </c>
+      <c r="G12" s="9">
         <v>1</v>
       </c>
+      <c r="H12" s="7" t="s">
+        <v>98</v>
+      </c>
       <c r="I12" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="M12" s="9">
+        <v>31</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L12" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:13">
+    <row r="13" spans="2:12">
       <c r="B13" s="5" t="s">
         <v>45</v>
       </c>
@@ -3651,52 +3588,48 @@
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-    </row>
-    <row r="14" spans="2:13">
+    </row>
+    <row r="14" spans="2:12">
       <c r="B14" s="8" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="9">
+        <v>97</v>
+      </c>
+      <c r="G14" s="9">
         <v>1</v>
       </c>
-      <c r="I14" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="M14" s="9">
+      <c r="H14" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="L14" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:13">
+    <row r="15" spans="2:12">
       <c r="B15" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D15" s="8">
         <v>111</v>
@@ -3705,36 +3638,33 @@
         <v>31</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="9">
+        <v>97</v>
+      </c>
+      <c r="G15" s="9">
         <v>1</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="H15" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="J15" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="J15" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="M15" s="9">
+      <c r="K15" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="L15" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:13">
+    <row r="16" spans="2:12">
       <c r="B16" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D16" s="8">
         <v>110</v>
@@ -3743,36 +3673,33 @@
         <v>31</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="9">
+        <v>97</v>
+      </c>
+      <c r="G16" s="9">
         <v>1</v>
       </c>
-      <c r="I16" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="M16" s="9">
+      <c r="H16" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="L16" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:13">
+    <row r="17" spans="2:12">
       <c r="B17" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D17" s="8">
         <v>100</v>
@@ -3781,183 +3708,168 @@
         <v>31</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="9">
+        <v>97</v>
+      </c>
+      <c r="G17" s="9">
         <v>1</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="M17" s="9">
+      <c r="H17" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="L17" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:13">
+    <row r="18" spans="2:12">
       <c r="B18" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="9">
+        <v>1</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" s="9">
-        <v>1</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="K18" s="7" t="s">
+      <c r="J18" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="K18" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="L18" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="M18" s="9">
+      <c r="L18" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:13">
+    <row r="19" spans="2:12">
       <c r="B19" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D19" s="8">
         <v>101</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" s="9">
+        <v>97</v>
+      </c>
+      <c r="G19" s="9">
         <v>1</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="M19" s="9">
+      <c r="H19" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="L19" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:13">
+    <row r="20" spans="2:12">
       <c r="B20" s="8" t="s">
         <v>54</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D20" s="8">
         <v>101</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="9">
+        <v>97</v>
+      </c>
+      <c r="G20" s="9">
         <v>1</v>
       </c>
-      <c r="I20" s="7" t="s">
-        <v>104</v>
+      <c r="H20" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="M20" s="9">
+        <v>116</v>
+      </c>
+      <c r="L20" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:13">
+    <row r="21" spans="2:12">
       <c r="B21" s="8" t="s">
         <v>55</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>31</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="9">
+        <v>97</v>
+      </c>
+      <c r="G21" s="9">
         <v>1</v>
       </c>
+      <c r="H21" s="8" t="s">
+        <v>119</v>
+      </c>
       <c r="I21" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="M21" s="8">
+        <v>115</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="L21" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:13">
+    <row r="22" spans="2:12">
       <c r="B22" s="8" t="s">
         <v>57</v>
       </c>
@@ -3965,37 +3877,34 @@
         <v>1100111</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E22" s="23" t="s">
         <v>31</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22" s="8">
+        <v>120</v>
+      </c>
+      <c r="G22" s="8">
         <v>1</v>
       </c>
+      <c r="H22" s="8" t="s">
+        <v>121</v>
+      </c>
       <c r="I22" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="M22" s="8">
+        <v>115</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="L22" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:13">
+    <row r="23" spans="2:12">
       <c r="B23" s="5" t="s">
         <v>59</v>
       </c>
@@ -4009,47 +3918,43 @@
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-    </row>
-    <row r="24" spans="2:13">
+    </row>
+    <row r="24" spans="2:12">
       <c r="B24" s="8" t="s">
         <v>60</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E24" s="23" t="s">
         <v>31</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="G24" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="8">
+        <v>97</v>
+      </c>
+      <c r="G24" s="8">
         <v>0</v>
       </c>
+      <c r="H24" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="I24" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="K24" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="L24" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="M24" s="8">
+        <v>123</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="L24" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:13">
+    <row r="25" spans="2:12">
       <c r="B25" s="5" t="s">
         <v>63</v>
       </c>
@@ -4063,9 +3968,8 @@
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-    </row>
-    <row r="26" spans="2:13">
+    </row>
+    <row r="26" spans="2:12">
       <c r="B26" s="8" t="s">
         <v>64</v>
       </c>
@@ -4073,37 +3977,34 @@
         <v>1100011</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E26" s="23" t="s">
         <v>31</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="H26" s="8">
+        <v>124</v>
+      </c>
+      <c r="G26" s="8">
         <v>0</v>
       </c>
+      <c r="H26" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="I26" s="8" t="s">
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="L26" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="M26" s="9">
+        <v>126</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L26" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:13">
+    <row r="27" spans="2:12">
       <c r="B27" s="8" t="s">
         <v>67</v>
       </c>
@@ -4111,39 +4012,36 @@
         <v>1100011</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>31</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="H27" s="8">
+        <v>124</v>
+      </c>
+      <c r="G27" s="8">
         <v>0</v>
       </c>
+      <c r="H27" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="I27" s="8" t="s">
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="L27" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="M27" s="9">
+        <v>127</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L27" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:13">
+    <row r="28" spans="2:12">
       <c r="B28" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" s="8">
         <v>1100011</v>
@@ -4155,33 +4053,30 @@
         <v>31</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="H28" s="8">
+        <v>124</v>
+      </c>
+      <c r="G28" s="8">
         <v>0</v>
       </c>
+      <c r="H28" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="I28" s="8" t="s">
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="L28" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="M28" s="9">
+        <v>128</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L28" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:13">
+    <row r="29" spans="2:12">
       <c r="B29" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C29" s="8">
         <v>1100011</v>
@@ -4193,33 +4088,30 @@
         <v>31</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="H29" s="8">
+        <v>124</v>
+      </c>
+      <c r="G29" s="8">
         <v>0</v>
       </c>
+      <c r="H29" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="I29" s="8" t="s">
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="L29" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="M29" s="9">
+        <v>129</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L29" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:13">
+    <row r="30" spans="2:12">
       <c r="B30" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -4231,14 +4123,13 @@
       <c r="J30" s="11"/>
       <c r="K30" s="11"/>
       <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-    </row>
-    <row r="31" spans="2:13">
+    </row>
+    <row r="31" spans="2:12">
       <c r="B31" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D31" s="23" t="s">
         <v>31</v>
@@ -4247,33 +4138,30 @@
         <v>31</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31" s="9">
+        <v>97</v>
+      </c>
+      <c r="G31" s="9">
         <v>1</v>
       </c>
-      <c r="I31" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>142</v>
+      <c r="H31" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="L31" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="M31" s="8">
+      <c r="L31" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:13">
+    <row r="32" spans="2:12">
       <c r="B32" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -4285,11 +4173,10 @@
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-    </row>
-    <row r="33" spans="2:13">
+    </row>
+    <row r="33" spans="2:12">
       <c r="B33" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C33" s="8">
         <v>1101111</v>
@@ -4301,33 +4188,30 @@
         <v>31</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H33" s="9">
+        <v>133</v>
+      </c>
+      <c r="G33" s="9">
         <v>1</v>
       </c>
+      <c r="H33" s="8" t="s">
+        <v>121</v>
+      </c>
       <c r="I33" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>144</v>
+        <v>134</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="L33" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="M33" s="8">
+      <c r="L33" s="8">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="F2:M2"/>
+    <mergeCell ref="F2:L2"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
@@ -4337,7 +4221,7 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="C31 C24:D24 D26:D29 E18:E20 D21:D22 C14:C22 C5:E12 D14 D18" numberStoredAsText="1"/>
+    <ignoredError sqref="D18 D14 C5:E12 C14:C22 D21:D22 E18:E20 D26:D29 C24:D24 C31" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>